<commit_message>
Updated BN, changed some code
CPT generator & leaflet map still don't work properly...
</commit_message>
<xml_diff>
--- a/data/raw/WWT_definitions_norway.xlsx
+++ b/data/raw/WWT_definitions_norway.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/346ebfb30976329f/Projects/Papers/03_Bayesian_Mixture_Toxicity/API_RQ_BN/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{97C86049-0877-4149-814A-824B0DBD7CFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{77D7EDE7-1A20-4F60-A40A-D734E8B46DF6}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{97C86049-0877-4149-814A-824B0DBD7CFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{36B4435D-65E2-4017-BC39-3F0438D4455A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{C3D78A78-6A2C-4CB2-A141-EE640EC20648}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +785,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -802,7 +802,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added more scenarios to BN, updated graphics
</commit_message>
<xml_diff>
--- a/data/raw/WWT_definitions_norway.xlsx
+++ b/data/raw/WWT_definitions_norway.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/346ebfb30976329f/Projects/Papers/03_Bayesian_Mixture_Toxicity/API_RQ_BN/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="8_{97C86049-0877-4149-814A-824B0DBD7CFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{36B4435D-65E2-4017-BC39-3F0438D4455A}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{97C86049-0877-4149-814A-824B0DBD7CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36B4435D-65E2-4017-BC39-3F0438D4455A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{C3D78A78-6A2C-4CB2-A141-EE640EC20648}"/>
+    <workbookView xWindow="30612" yWindow="-6792" windowWidth="17496" windowHeight="30336" xr2:uid="{C3D78A78-6A2C-4CB2-A141-EE640EC20648}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,6 +236,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,7 +542,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>